<commit_message>
update to remmove guid
</commit_message>
<xml_diff>
--- a/my_data.xlsx
+++ b/my_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,45 +471,35 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 19</t>
+          <t>concat_update_judul</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 20</t>
+          <t>concat_update_tipe_kewajiban</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>concat_update_judul</t>
+          <t>concat_update_sanksi</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>concat_update_tipe_kewajiban</t>
+          <t>concat_update_checklist</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>concat_update_sanksi</t>
+          <t>concat_update_peraturan_kewajiban</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>concat_update_checklist</t>
+          <t>concat_update_peraturan_sanksi</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>concat_update_peraturan_kewajiban</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>concat_update_peraturan_sanksi</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>hash</t>
         </is>
@@ -517,16 +507,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pertambangan Batubara&gt;Tenaga Kerja Bidang Pertambangan Batubara&gt;Ketentuan Umum Tenaga Kerja di Bidang Pertambangan Batubara</t>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mengutamakan penggunaan tenaga kerja setempat, bagi Pemegang IUP Eksplorasi, IUPK Eksplorasi, IUP Operasi Produksi, IUPK Operasi Produksi, dan IUP Operasi Produksi khusus untuk pengolahan dan/atau pemurnian</t>
+          <t>Memenuhi komitmen Tingkat Komponen Dalam Negeri (TKDN) jasa yang dinyatakan sendiri (self-assesment) dan ditetapkan dalam kontrak, bagi Produsen Dalam Negeri dan Penyedia Barang dan/atau Jasa</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -541,109 +531,1307 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1. Menyusun dan membiayai program pendidikan dan pelatihan tenaga kerja setempat dan/atau nasional</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Peraturan Pemerintah Nomor 96 Tahun 2021@lt614815d4f1925
+          <t>Peraturan Menteri Energi Dan Sumber Daya Mineral Nomor 15 Tahun 2013@lt5135ade06c682
 Kewajiban
-Pasal 161 &gt;&gt;&gt; @lt614815d4f1925
-(1) Pemegang IUP dan IUPK wajib mengutamakan penggunaan tenaga kerja setempat.
-(2) Dalam hal tidak tersedia tenaga kerja setempat sebagaimana dimaksud pada ayat (1) yang memiliki kompetensi dan keahlian, pemegang IUP dan IUPK dapat menggunakan tenaga kerja nasional.
-(3) Dalam hal tidak tersedia tenaga kerja nasionai sebagainrana dimaksud pada ayat (2) yang memiliki kompetensi dan keahlian, pemegang IUP dan IUPK dapat menggunakan tenaga kerja asing setelah mendapatkan persetujuan dari instansi yang menyelenggarakan urusan pemerintahan di bidang ketenagakerjaan.
-Peraturan Menteri Energi Dan Sumber Daya Mineral Nomor 25 Tahun 2018@lt5af950ccbfc3d
+Pasal 8
+(1) Dalam upaya mengutamakan penggunaan Produk Dalam Negeri, Produsen Dalam Negeri dan/atau Penyedia Barang dan/atau Jasa wajib:
+[...]
+b. memenuhi komitmen TKDN jasa yang dinyatakan sendiri (self assesment) yang ditetapkan di dalam kontrak pengadaan barang dan/atau jasa;
+[...]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Peraturan Menteri Energi Dan Sumber Daya Mineral Nomor 15 Tahun 2013@lt5135ade06c682
+Sanksi
+Pasal 22
+(1) Produsen Dalam Negeri yang melanggar ketentuan dalam [...], Pasal 8 ayat (1) huruf b, [...] dikenai sanksi administratif oleh Direktur Jenderal berupa teguran tertulis dan/atau pencabutan SKUP Migas.
+(2) Penyedia Barang dan/atau Jasa yang melanggar ketentuan dalam [...], Pasal 8 ayat (1) huruf b, [...] dikenai sanksi administratif oleh Direktur Jenderal berupa teguran tertulis dan/atau pencabutan SKUP Migas.
+(3) Sanksi administratif berupa teguran tertulis sebagaimana dimaksud pada ayat (1) dan ayat (2) diberikan paling banyak 2 (dua) kali masing-masing dalam jangka waktu paling lama 1 (satu) bulan.
+(4) Dalam hal Produsen Dalam Negeri atau Penyedia Barang dan/atau Jasa yang mendapat teguran tertulis setelah berakhirnya jangka waktu teguran tertulis kedua sebagaimana dimaksud pada ayat (3) tidak melaksanakan kewajibannya, maka Direktur Jenderal mengenakan sanksi administratif berupa pencabutan SKUP Migas.
+Pasal 23
+(1) Produsen Dalam Negeri dan/atau Penyedia Barang dan/atau Jasa yang melanggar ketentuan dalam Pasal 8 ayat (1) butir b, [...] setelah pelaksanaan kontrak pengadaan barang dan/atau jasa, dikenai sanksi finansial oleh Kontraktor dengan ketentuan sebagai berikut:
+a. apabila tidak mengubah peringkat pemenang, besarnya sanksi adalah selisih antara Harga Evaluasi Penawaran (HEP) tahap realisasi kontrak dan Harga Evaluasi Penawaran (HEP) tahap penawaran;
+b. apabila mengubah peringkat pemenang, besarnya sanksi adalah selisih antara Harga Evaluasi Penawaran (HEP) tahap realisasi kontrak dan Harga Evaluasi Penawaran (HEP) tahap penawaran, ditambah selisih antara nilai kontrak peringkat I dan nilai penawaran peringkat II pada tahap penawaran.
+(2) Sanksi finansial sebagaimana dimaksud pada ayat (1) dikurangkan dari nilai pembayaran kontrak.
+(3) Contoh perhitungan besarnya sanksi sebagaimana dimaksud pada ayat (2) adalah sebagaimana tercantum dalam Lampiran V yang merupakan bagian yang tidak terpisahkan dari Peraturan Menteri ini.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>memenuhikomitmentingkatkomponendalamnegeri(tkdn)jasayangdinyatakansendiri(self-assesment)danditetapkandalamkontrak,bagiprodusendalamnegeridanpenyediabarangdan/ataujasa</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>continuous</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>peraturanmenterienergidansumberdayamineralnomor15tahun2013kewajibanpasal8(1)dalamupayamengutamakanpenggunaanprodukdalamnegeri,produsendalamnegeridan/ataupenyediabarangdan/ataujasawajib:[...]b.memenuhikomitmentkdnjasayangdinyatakansendiri(selfassesment)yangditetapkandidalamkontrakpengadaanbarangdan/ataujasa;[...]</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>peraturanmenterienergidansumberdayamineralnomor15tahun2013sanksipasal22(1)produsendalamnegeriyangmelanggarketentuandalam[...],pasal8ayat(1)hurufb,[...]dikenaisanksiadministratifolehdirekturjenderalberupategurantertulisdan/ataupencabutanskupmigas.(2)penyediabarangdan/ataujasayangmelanggarketentuandalam[...],pasal8ayat(1)hurufb,[...]dikenaisanksiadministratifolehdirekturjenderalberupategurantertulisdan/ataupencabutanskupmigas.(3)sanksiadministratifberupategurantertulissebagaimanadimaksudpadaayat(1)danayat(2)diberikanpalingbanyak2(dua)kalimasing-masingdalamjangkawaktupalinglama1(satu)bulan.(4)dalamhalprodusendalamnegeriataupenyediabarangdan/ataujasayangmendapattegurantertulissetelahberakhirnyajangkawaktutegurantertuliskeduasebagaimanadimaksudpadaayat(3)tidakmelaksanakankewajibannya,makadirekturjenderalmengenakansanksiadministratifberupapencabutanskupmigas.pasal23(1)produsendalamnegeridan/ataupenyediabarangdan/ataujasayangmelanggarketentuandalampasal8ayat(1)butirb,[...]setelahpelaksanaankontrakpengadaanbarangdan/ataujasa,dikenaisanksifinansialolehkontraktordenganketentuansebagaiberikut:a.apabilatidakmengubahperingkatpemenang,besarnyasanksiadalahselisihantarahargaevaluasipenawaran(hep)tahaprealisasikontrakdanhargaevaluasipenawaran(hep)tahappenawaran;b.apabilamengubahperingkatpemenang,besarnyasanksiadalahselisihantarahargaevaluasipenawaran(hep)tahaprealisasikontrakdanhargaevaluasipenawaran(hep)tahappenawaran,ditambahselisihantaranilaikontrakperingkatidannilaipenawaranperingkatiipadatahappenawaran.(2)sanksifinansialsebagaimanadimaksudpadaayat(1)dikurangkandarinilaipembayarankontrak.(3)contohperhitunganbesarnyasanksisebagaimanadimaksudpadaayat(2)adalahsebagaimanatercantumdalamlampiranvyangmerupakanbagianyangtidakterpisahkandariperaturanmenteriini.</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>5b43d12c6279cae1412425c0d6a48c146a5914fa72a5cd777a27f6d858771b30</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mendapatkan persetujuan dari SKK Migas untuk Daftar Pengadaan (Procurement List) dalam tahap Eksplorasi, dengan nilai Paket Tender lebih dari Rp50.000.000.000,00 (lima puluh miliar rupiah), sebagai bagian dari Work Program and Budget (WP&amp;B) pada setiap tahun anggaran</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Licensing</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Menyusun Daftar Pengadaan (Procurement List) yang berisi informasi status Kontrak dan/atau Paket Tender, antara lain: a. Kontrak yang sedang berjalan (active); b. Paket Tender yang proses Tender-nya sedang berjalan (ongoing); c. Paket Tender yang proses Tender-nya akan dilaksanakan pada tahun yang bersangkutan atau berikutnya (future); d. Kontrak yang telah selesai dilaksanakan pada tahun sebelumnya (completed); dan e. Paket Tender yang dibatalkan (canceled).</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>mendapatkanpersetujuandariskkmigasuntukdaftarpengadaan(procurementlist)dalamtahapeksplorasi,dengannilaipakettenderlebihdarirp50.000.000.000,00(limapuluhmiliarrupiah),sebagaibagiandariworkprogramandbudget(wp&amp;b)padasetiaptahunanggaran</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>licensing</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>menyusundaftarpengadaan(procurementlist)yangberisiinformasistatuskontrakdan/ataupakettender,antaralain:a.kontrakyangsedangberjalan(active);b.pakettenderyangprosestender-nyasedangberjalan(ongoing);c.pakettenderyangprosestender-nyaakandilaksanakanpadatahunyangbersangkutanatauberikutnya(future);d.kontrakyangtelahselesaidilaksanakanpadatahunsebelumnya(completed);dane.pakettenderyangdibatalkan(canceled).</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>7486d0394521407582b95f14dab2a0cd7500fc6c35859600fa500e77fdbd5d8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mengajukan permohonan persetujuan Rencana Tender kepada SKK Migas dalam jangka waktu 6 (enam) bulan sejak Prakualifikasi disetujui</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Licensing</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>mengajukanpermohonanpersetujuanrencanatenderkepadaskkmigasdalamjangkawaktu6(enam)bulansejakprakualifikasidisetujui</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>licensing</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>b1425f304693fcacd879cd8adf76c6a64ec243267f9890faf9eaee498b14a55a</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Melakukan pembayaran kepada Penyedia Barang/Jasa dalam tahap Eksploitasi melalui bank Badan Usaha Milik Negara (BUMN)/Daerah (BUMD)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
 Kewajiban
-Pasal 29 &gt;&gt;&gt; @lt5af950ccbfc3d
-(1) Pemegang IUP Eksplorasi, IUPK Eksplorasi, IUP Operasi Produksi, IUPK Operasi Produksi, IUP Operasi Produksi khusus untuk pengolahan dan/atau pemurnian, dan Izin Usaha Jasa Pertambangan wajib mengutamakan tenaga kerja setempat dan/atau nasional.
-[...]
-(3) Pemegang IUP Eksplorasi, IUPK Eksplorasi, IUP Operasi Produksi, IUPK Operasi Produksi, IUP Operasi Produksi khusus untuk pengolahan dan/atau pemurnian, dan Izin Usaha Jasa Pertambangan wajib menyusun dan membiayai program pendidikan dan pelatihan tenaga kerja setempat dan/atau nasional.
-Peraturan Menteri Energi Dan Sumber Daya Mineral Nomor 39 Tahun 2008@lt575fd38089bab
+LAMPIRAN
+BAB IV
+1. Ketentuan Umum
+1.7. KKKS Cost Recovery dalam tahap eksploitasi wajib melaksanakan pembayaran kepada Pelaksana Kontrak menggunakan Bank BUMN/BUMD. KKKS Cost Recovery dalam tahap eksplorasi, dapat melaksanakan pembayaran menggunakan Bank BUMN/BUMD atau Bank Umum Swasta Nasional. Ketentuan ini dikecualikan untuk pelaksanaan pembayaran kepada Pelaksana Kontrak yang berstatus Perusahaan Asing.
+Surat Edaran Kepala BPMIGAS Nomor EDR-0067/BP00000/2008/SO Tahun 2008@28938
 Kewajiban
-Pasal 3 &gt;&gt;&gt; @lt575fd38089bab
-Dalam melaksanakan kegiatan usaha pertambangan mineral dan batubara, pemegang Kuasa Pertambangan, pemegang Kontrak Karya dan pemegang Perjanjian Karya Pengusahaan Pertambangan Batubara wajib mempekerjakan tenaga kerja yang memiliki sertifikat kompetensi kerja sesuai SKKNI sebagaimana dimaksud dalam Pasal 1.</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Peraturan Pemerintah Nomor 96 Tahun 2021@lt614815d4f1925
+1. Kontraktor Kontrak Kerja Sama (“KKKS”) harus mengutamakan penggunaan Bank Umum Nasional dalam melakukan pembayaran kepada Penyedia Barang/Jasa baik untuk rekening pembayar maupun rekening penerima sebagaimana telah dirubah dalam Surat Keputusan Kepala BPMIGAS Nomor KEP- 0066/BP00000/2008/SO tentang Pelaksanaan Pengadaan Barang/Jasa yang mengubah isi Bab I huruf C angka 2 dan Bab III huruf A angka 9 a, PTK No.007/PTK/VI/2004 tentang Pengelolaan Rantai Suplai KKKS.
+2. Yang dimaksud dengan Penyedia Barang/Jasa dalam surat edaran ini adalah sebagaimana dinyatakan dalam PTK No.007/PTK/VI/2004 tentang Pengelolaan Rantai Suplai KKKS Buku II Bab l Huruf A 10.
+3. KKKS harus mengutamakan penggunaan Bank Umum Nasional dalam penggunaan jasa perbankan lain terkait kegiatan usaha hulu minyak dan gas bumi.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
 Sanksi
-Pasal 185 &gt;&gt;&gt; @lt614815d4f1925
-(1) Pemegang IUP, IUPK, IPR, SIPB, atau IUP untuk Penjualan yang melakukan pelanggaran terhadap ketentuan sebagaimana dimaksud dalam […] Pasal 161 ayat (1) […] dikenai sanksi administratif.
-(2) sanksi administratif sebagaimana dimaksud pada ayat (1) benrpa:
-a. peringatan tertulis;
-b. penghentian sernentara sebagian atau seluruh kegiatan Eksplorasi atau Operasi produksi; dan/atau
-c. pencabutan IUP, IUPK, IPR, SIPB, atau IUP untuk Penjualan.
-(3) selain sanksi administratif sebagaimana dimaksud pada ayat (2), pemegang IUP, IUPK, IPR, atau SIPB, yang melakukan pelanggaran terhadap ketentuan sebagaimana dimaksud dalam pasal 51 ayat (2) huruf b dan Pasal 107 ayat (2) huruf b dikenai denda.
-(4) Pengenaan denda sebagaimana dimaksud pada ayat (3) dilaksanakan sesuai dengan ketentuan peraturan perundang-undangan di bidang pajak daerah dan retribusi daerah.
-Pasal 186 &gt;&gt;&gt; @lt614815d4f1925
-Peringatan tertulis sebagaimana dimaksud dalam pasal 185 ayat (2) huruf a diberikan paling banyak 3 (tiga) kali dengan jangka waktu peringatan masing-masing 30 (tiga puluh) hari kalender.
-Peraturan Menteri Energi dan Sumber Daya Mineral Nomor 7 Tahun 2020@lt5e6f51a775ad4
+LAMPIRAN
+BAB X
+1. Pengawasan Terhadap KKKS Cost Recovery
+1.2. Sanksi atas pelanggaran dalam pengelolaan Pengadaan Barang/Jasa berdasarkan hasil audit adalah sebagai berikut:
+1.2.1. Sanksi administrasi
+Berupa surat peringatan kepada pimpinan tertinggi KKKS Cost Recovery, jika:
+1.2.1.1. Tidak melaksanakan proses pengelolaan Pengadaan Barang/Jasa sesuai dengan ketentuan pedoman ini, Petunjuk Pelaksanaan Pengadaan Barang/Jasa, Dokumen Tender, dan/atau Kontrak;
+BAB XII
+3. Apabila KKKS Cost Recovery terbukti melakukan kelalaian, kesalahan, atau pelanggaran terhadap Peraturan Perundang-Undangan yang berlaku, maka KKKS Cost Recovery bertanggung jawab atas segala akibat hukum yang timbul dan melepaskan, membebaskan, dan membela SKK Migas dari dan terhadap setiap kerugian, tuntutan, dan gugatan hukum pihak ketiga sebagai akibat dari kelalaian, kesalahan, atau pelanggaran kewajiban hukum KKKS Cost Recovery terhadap Peraturan Perundang-Undangan yang berlaku.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>melakukanpembayarankepadapenyediabarang/jasadalamtahapeksploitasimelaluibankbadanusahamiliknegara(bumn)/daerah(bumd)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>continuous</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023kewajibanlampiranbabiv1.ketentuanumum1.7.kkkscostrecoverydalamtahapeksploitasiwajibmelaksanakanpembayarankepadapelaksanakontrakmenggunakanbankbumn/bumd.kkkscostrecoverydalamtahapeksplorasi,dapatmelaksanakanpembayaranmenggunakanbankbumn/bumdataubankumumswastanasional.ketentuaninidikecualikanuntukpelaksanaanpembayarankepadapelaksanakontrakyangberstatusperusahaanasing.suratedarankepalabpmigasnomoredr-0067/bp00000/2008/sotahun2008@28938kewajiban1.kontraktorkontrakkerjasama(“kkks”)harusmengutamakanpenggunaanbankumumnasionaldalammelakukanpembayarankepadapenyediabarang/jasabaikuntukrekeningpembayarmaupunrekeningpenerimasebagaimanatelahdirubahdalamsuratkeputusankepalabpmigasnomorkep-0066/bp00000/2008/sotentangpelaksanaanpengadaanbarang/jasayangmengubahisibabihurufcangka2danbabiiihurufaangka9a,ptkno.007/ptk/vi/2004tentangpengelolaanrantaisuplaikkks.2.yangdimaksuddenganpenyediabarang/jasadalamsuratedaraniniadalahsebagaimanadinyatakandalamptkno.007/ptk/vi/2004tentangpengelolaanrantaisuplaikkksbukuiibablhurufa10.3.kkksharusmengutamakanpenggunaanbankumumnasionaldalampenggunaanjasaperbankanlainterkaitkegiatanusahahuluminyakdangasbumi.</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023sanksilampiranbabx1.pengawasanterhadapkkkscostrecovery1.2.sanksiataspelanggarandalampengelolaanpengadaanbarang/jasaberdasarkanhasilauditadalahsebagaiberikut:1.2.1.sanksiadministrasiberupasuratperingatankepadapimpinantertinggikkkscostrecovery,jika:1.2.1.1.tidakmelaksanakanprosespengelolaanpengadaanbarang/jasasesuaidenganketentuanpedomanini,petunjukpelaksanaanpengadaanbarang/jasa,dokumentender,dan/ataukontrak;babxii3.apabilakkkscostrecoveryterbuktimelakukankelalaian,kesalahan,ataupelanggaranterhadapperaturanperundang-undanganyangberlaku,makakkkscostrecoverybertanggungjawabatassegalaakibathukumyangtimbuldanmelepaskan,membebaskan,danmembelaskkmigasdaridanterhadapsetiapkerugian,tuntutan,dangugatanhukumpihakketigasebagaiakibatdarikelalaian,kesalahan,ataupelanggarankewajibanhukumkkkscostrecoveryterhadapperaturanperundang-undanganyangberlaku.</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>93b5218837dafd40a2d82bc1cb0035bec5fc596ac013b3492e572b635c25a7c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Melakukan pembayaran kepada Penyedia Barang/Jasa dalam tahap Eksplorasi melalui bank Badan Usaha Milik Negara (BUMN)/Daerah (BUMD), atau bank umum swasta nasional</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
+Kewajiban
+LAMPIRAN
+BAB IV
+1. Ketentuan Umum
+1.7. KKKS Cost Recovery dalam tahap eksploitasi wajib melaksanakan pembayaran kepada Pelaksana Kontrak menggunakan Bank BUMN/BUMD. KKKS Cost Recovery dalam tahap eksplorasi, dapat melaksanakan pembayaran menggunakan Bank BUMN/BUMD atau Bank Umum Swasta Nasional. Ketentuan ini dikecualikan untuk pelaksanaan pembayaran kepada Pelaksana Kontrak yang berstatus Perusahaan Asing.
+Surat Edaran Kepala BPMIGAS Nomor EDR-0067/BP00000/2008/SO Tahun 2008@28938
+Kewajiban
+1. Kontraktor Kontrak Kerja Sama (“KKKS”) harus mengutamakan penggunaan Bank Umum Nasional dalam melakukan pembayaran kepada Penyedia Barang/Jasa baik untuk rekening pembayar maupun rekening penerima sebagaimana telah dirubah dalam Surat Keputusan Kepala BPMIGAS Nomor KEP- 0066/BP00000/2008/SO tentang Pelaksanaan Pengadaan Barang/Jasa yang mengubah isi Bab I huruf C angka 2 dan Bab III huruf A angka 9 a, PTK No.007/PTK/VI/2004 tentang Pengelolaan Rantai Suplai KKKS.
+2. Yang dimaksud dengan Penyedia Barang/Jasa dalam surat edaran ini adalah sebagaimana dinyatakan dalam PTK No.007/PTK/VI/2004 tentang Pengelolaan Rantai Suplai KKKS Buku II Bab l Huruf A 10.
+3. KKKS harus mengutamakan penggunaan Bank Umum Nasional dalam penggunaan jasa perbankan lain terkait kegiatan usaha hulu minyak dan gas bumi.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
 Sanksi
-Pasal 95 
-(1) Pemegang IUP, IUPK, IUP Operasi Produksi khusus untuk pengolahan dan/atau pemurnian, IUJP, dan IUP Operasi Produksi khusus untuk pengangkutan dan penjualan, yang tidak mematuhi atau melanggar ketentuan sebagaimana dimaksud dalam [...] Pasal 72 huruf a atau huruf m [...].
-(2) Sanksi administratif sebagaimana dimaksud pada ayat (1) berupa:
-a. peringatan tertulis;
-b. penghentian sementara sebagian atau seluruh kegiatan usaha; dan/atau
-c. pencabutan izin.
-(3) Sanksi administratif sebagaimana dimaksud pada ayat (2) diberikan oleh Direktur Jenderal atas nama Menteri atau gubernur sesuai dengan kewenangannya.
-Peraturan Menteri Energi Dan Sumber Daya Mineral Nomor 25 Tahun 2018@lt5af950ccbfc3d
+LAMPIRAN
+BAB X
+1. Pengawasan Terhadap KKKS Cost Recovery
+1.2. Sanksi atas pelanggaran dalam pengelolaan Pengadaan Barang/Jasa berdasarkan hasil audit adalah sebagai berikut:
+1.2.1. Sanksi administrasi
+Berupa surat peringatan kepada pimpinan tertinggi KKKS Cost Recovery, jika:
+1.2.1.1. Tidak melaksanakan proses pengelolaan Pengadaan Barang/Jasa sesuai dengan ketentuan pedoman ini, Petunjuk Pelaksanaan Pengadaan Barang/Jasa, Dokumen Tender, dan/atau Kontrak;
+BAB XII
+3. Apabila KKKS Cost Recovery terbukti melakukan kelalaian, kesalahan, atau pelanggaran terhadap Peraturan Perundang-Undangan yang berlaku, maka KKKS Cost Recovery bertanggung jawab atas segala akibat hukum yang timbul dan melepaskan, membebaskan, dan membela SKK Migas dari dan terhadap setiap kerugian, tuntutan, dan gugatan hukum pihak ketiga sebagai akibat dari kelalaian, kesalahan, atau pelanggaran kewajiban hukum KKKS Cost Recovery terhadap Peraturan Perundang-Undangan yang berlaku.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>melakukanpembayarankepadapenyediabarang/jasadalamtahapeksplorasimelaluibankbadanusahamiliknegara(bumn)/daerah(bumd),ataubankumumswastanasional</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>continuous</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023kewajibanlampiranbabiv1.ketentuanumum1.7.kkkscostrecoverydalamtahapeksploitasiwajibmelaksanakanpembayarankepadapelaksanakontrakmenggunakanbankbumn/bumd.kkkscostrecoverydalamtahapeksplorasi,dapatmelaksanakanpembayaranmenggunakanbankbumn/bumdataubankumumswastanasional.ketentuaninidikecualikanuntukpelaksanaanpembayarankepadapelaksanakontrakyangberstatusperusahaanasing.suratedarankepalabpmigasnomoredr-0067/bp00000/2008/sotahun2008@28938kewajiban1.kontraktorkontrakkerjasama(“kkks”)harusmengutamakanpenggunaanbankumumnasionaldalammelakukanpembayarankepadapenyediabarang/jasabaikuntukrekeningpembayarmaupunrekeningpenerimasebagaimanatelahdirubahdalamsuratkeputusankepalabpmigasnomorkep-0066/bp00000/2008/sotentangpelaksanaanpengadaanbarang/jasayangmengubahisibabihurufcangka2danbabiiihurufaangka9a,ptkno.007/ptk/vi/2004tentangpengelolaanrantaisuplaikkks.2.yangdimaksuddenganpenyediabarang/jasadalamsuratedaraniniadalahsebagaimanadinyatakandalamptkno.007/ptk/vi/2004tentangpengelolaanrantaisuplaikkksbukuiibablhurufa10.3.kkksharusmengutamakanpenggunaanbankumumnasionaldalampenggunaanjasaperbankanlainterkaitkegiatanusahahuluminyakdangasbumi.</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023sanksilampiranbabx1.pengawasanterhadapkkkscostrecovery1.2.sanksiataspelanggarandalampengelolaanpengadaanbarang/jasaberdasarkanhasilauditadalahsebagaiberikut:1.2.1.sanksiadministrasiberupasuratperingatankepadapimpinantertinggikkkscostrecovery,jika:1.2.1.1.tidakmelaksanakanprosespengelolaanpengadaanbarang/jasasesuaidenganketentuanpedomanini,petunjukpelaksanaanpengadaanbarang/jasa,dokumentender,dan/ataukontrak;babxii3.apabilakkkscostrecoveryterbuktimelakukankelalaian,kesalahan,ataupelanggaranterhadapperaturanperundang-undanganyangberlaku,makakkkscostrecoverybertanggungjawabatassegalaakibathukumyangtimbuldanmelepaskan,membebaskan,danmembelaskkmigasdaridanterhadapsetiapkerugian,tuntutan,dangugatanhukumpihakketigasebagaiakibatdarikelalaian,kesalahan,ataupelanggarankewajibanhukumkkkscostrecoveryterhadapperaturanperundang-undanganyangberlaku.</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>9ad5b9f683fe90fe94ab3f49a87c037a8e406ab7016d1352979af687431b04e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Menggunakan e-Catalog dalam hal SKK Migas telah mengembangkan e-Catalog untuk komoditas tertentu</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Conditional</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>menggunakane-catalogdalamhalskkmigastelahmengembangkane-cataloguntukkomoditastertentu</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>conditional</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>7412b64dba8e3e271f6b168f50aec9298862d9d613f69824689ae60c3c12ac42</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Melakukan konsolidasi data dan menyiapkan laporan berkala terkait dengan manajemen Kontrak</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>melakukankonsolidasidatadanmenyiapkanlaporanberkalaterkaitdenganmanajemenkontrak</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>continuous</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>b00526511fc474059e29b2274cfb6ca693366f5bc4dd33340f508ecf03ab4d95</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mengenakan sanksi berupa denda atas keterlambatan penyerahan barang atau pekerjaan</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>mengenakansanksiberupadendaatasketerlambatanpenyerahanbarangataupekerjaan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>continuous</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>a2e7f07072f5ddc5b0967bc9492f8c8d3ca250b0b6a6610f7797e4426710258c</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Mendapatkan persetujuan dari SKK Migas untuk menginisiasi pemeriksaan kepatuhan Penyedia Barang/Jasa terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan Anti-bribery and Corruption (ABC) yang dilakukan oleh auditor independen</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Licensing</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Menyampaikan pemberitahuan mengenai auditor independen yang ditunjuk kepada Penyedia Barang/Jasa.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
+Kewajiban
+LAMPIRAN
+BAB IX
+2. Pengawasan Penyedia Barang/Jasa
+Pengawasan berupa pemeriksaan dilakukan oleh KKKS Cost Recovery, SKK Migas atau auditor yang ditunjuk oleh SKK Migas secara current dan post audit, termasuk namun tidak terbatas pada kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan/atau Anti-Bribery and Corruption (ABC) berdasarkan data hardcopy dan data digital.
+2.2. Pemeriksaan kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, FCPA, dan/atau ABC dapat dilakukan oleh auditor independen dengan ketentuan:
+2.2.1. Apabila diinisiasi oleh KKKS Cost Recovery, maka harus mendapatkan persetujuan SKK Migas;
+2.2.2. Apabila diinisiasi oleh SKK Migas, maka SKK Migas akan memberitahukan dan melibatkan KKKS Cost Recovery;
+2.2.3. SKK Migas atau KKKS Cost Recovery memberitahukan kepada Pelaksana Kontrak mengenai auditor independen yang ditunjuk, dan Pelaksana Kontrak harus menyampaikan data hardcopy dan data digital kepada auditor independen tersebut; dan
+2.2.4. Biaya pemeriksaan dapat dibebankan sebagai biaya operasi berdasarkan KKS.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
 Sanksi
-Pasal 40 &gt;&gt;&gt; @lt5af950ccbfc3d
-(1)  Pemegang IUP Eksplorasi, IUPK Eksplorasi, IUP Operasi Produksi, IUPK Operasi Produksi, IUP Operasi Produksi khusus untuk pengolahan dan atau pemurnian, IUP Operasi Produksi khusus untuk pengangkutan dan penjualan, dan Izin Usaha Jasa Pertambangan yang tidak mematuhi atau melanggar ketentuan sebagaimana dimaksud dalam Pasal 8 ayat (1) atau sampai dengan ayat (3), Pasal 9 ayat (1), Pasal 10 ayat (1), Pasal 11 ayat (1), Pasal 12 ayat (1), Pasal 13, Pasal 14 ayat (1) atau ayat (3), Pasal 16 ayat (1) atau ayat (6), Pasal 17 ayat (1), Pasal 18 ayat (1) atau sampai dengan ayat (6), Pasal 22, Pasal 24 ayat (1) atau ayat (3), Pasal 25 ayat (1), Pasal 26 ayat (1) atau ayat (2), Pasal 27 ayat (1), Pasal 29 ayat (1) atau ayat (3), Pasal 30 ayat (1) atau ayat (4), Pasal 33 ayat (1),  Pasal 38 ayat (1), ayat (4), ayat (6), atau ayat (7), atau Pasal 39 ayat (1) dikenakan sanksi administratif.
-(2) Sanksi administratif sebagaimana dimaksud pada ayat (1) berupa:
-a. peringatan tertulis;
-b. penghentian sementara sebagian atau seluruh kegiatan usaha; dan/atau
-c. pencabutan izin.
-(3)  Sanksi administratif sebagaimana dimaksud pada ayat (2) diberikan oleh Direktur Jenderal atas nama Menteri atau gubernur sesuai dengan kewenangannya.
-Pasal 41 &gt;&gt;&gt; @lt5af950ccbfc3d
-Peringatan tertulis sebagaimana dimaksud dalam Pasal 40 ayat (2) huruf a diberikan paling banyak 3 (tiga) kali dengan jangka waktu peringatan masing-masing paling lama 30 (tiga puluh) hari kalender.
-Pasal 42 &gt;&gt;&gt; @lt5af950ccbfc3d
-(1) Dalam hal pemegang IUP Eksplorasi, IUPK Eksplorasi, IUP Operasi Produksi, IUPK Operasi Produksi, IUP Operasi Produksi khusus untuk pengolahan dan/atau pemurnian, IUP Operasi Produksi khusus untuk pengangkutan dan penjualan, atau Izin Usaha Jasa Pertambangan yang mendapat sanksi peringatan tertulis setelah berakhirnya jangka waktu peringatan tertulis sebagaimana dimaksud dalam Pasal 40 ayat (2) huruf a belum melaksanakan kewajibannya, dikenakan sanksi administratif berupa penghentian sementara sebagian atau seluruh kegiatan usaha sebagaimana dimaksud dalam Pasal 40 ayat (2) huruf b.
-(2) Sanksi administratif berupa penghentian sementara sebagian atau seluruh kegiatan usaha sebagaimana dimaksud pada ayat (1) dikenakan paling lama 60 (enam puluh) hari kalender.
-Pasal 43 &gt;&gt;&gt; @lt5af950ccbfc3d
-Sanksi administratif berupa pencabutan izin sebagaimana dimaksud dalam Pasal 40 ayat (2) huruf c dikenakan kepada pemegang IUP Eksplorasi, IUPK Eksplorasi, IUP Operasi Produksi, IUPK Operasi Produksi, IUP Operasi Produksi khusus untuk pengolahan dan/atau pemurnian, IUP Operasi Produksi khusus untuk pengangkutan dan penjualan, atau Izin Usaha Jasa Pertambangan yang tidak melaksanakan kewajiban sampai dengan berakhirnya jangka waktu pengenaan sanksi berupa penghentian sementara sebagian atau seluruh kegiatan usaha sebagaimana dimaksud dalam Pasal 42 ayat (2) huruf b.</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>1774</v>
-      </c>
-      <c r="J2" t="n">
-        <v>4886</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>mengutamakanpenggunaantenagakerjasetempat,bagipemegangiupeksplorasi,iupkeksplorasi,iupoperasiproduksi,iupkoperasiproduksi,daniupoperasiproduksikhususuntukpengolahandan/ataupemurnian</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
+LAMPIRAN
+BAB X
+1. Pengawasan Terhadap KKKS Cost Recovery
+1.2. Sanksi atas pelanggaran dalam pengelolaan Pengadaan Barang/Jasa berdasarkan hasil audit adalah sebagai berikut:
+1.2.1. Sanksi administrasi
+Berupa surat peringatan kepada pimpinan tertinggi KKKS Cost Recovery, jika:
+1.2.1.1. Tidak melaksanakan proses pengelolaan Pengadaan Barang/Jasa sesuai dengan ketentuan pedoman ini, Petunjuk Pelaksanaan Pengadaan Barang/Jasa, Dokumen Tender, dan/atau Kontrak;
+1.2.2. Sanksi finansial
+Tidak dapat dibebankan sebagai biaya operasi berdasarkan KKS pada periode perhitungan berikutnya atau setelah wilayah kerja KKKS Cost Recovery dalam tahap eksplorasi dinyatakan komersial untuk dikembangkan, untuk:
+1.2.2.2. Seluruh nilai Kontrak yang terealisasi, jika:
+1.2.2.2.5. Pelaksana Kontrak tidak bersedia dilakukan audit kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan/atau Anti-Bribery and Corruption (ABC) untuk Pengadaan Barang/Jasa dari Kontrak dimaksud.
+BAB XII
+3. Apabila KKKS Cost Recovery terbukti melakukan kelalaian, kesalahan, atau pelanggaran terhadap Peraturan Perundang-Undangan yang berlaku, maka KKKS Cost Recovery bertanggung jawab atas segala akibat hukum yang timbul dan melepaskan, membebaskan, dan membela SKK Migas dari dan terhadap setiap kerugian, tuntutan, dan gugatan hukum pihak ketiga sebagai akibat dari kelalaian, kesalahan, atau pelanggaran kewajiban hukum KKKS Cost Recovery terhadap Peraturan Perundang-Undangan yang berlaku.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>mendapatkanpersetujuandariskkmigasuntukmenginisiasipemeriksaankepatuhanpenyediabarang/jasaterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dananti-briberyandcorruption(abc)yangdilakukanolehauditorindependen</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>licensing</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>menyampaikanpemberitahuanmengenaiauditorindependenyangditunjukkepadapenyediabarang/jasa.</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023kewajibanlampiranbabix2.pengawasanpenyediabarang/jasapengawasanberupapemeriksaandilakukanolehkkkscostrecovery,skkmigasatauauditoryangditunjukolehskkmigassecaracurrentdanpostaudit,termasuknamuntidakterbataspadakepatuhanterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dan/atauanti-briberyandcorruption(abc)berdasarkandatahardcopydandatadigital.2.2.pemeriksaankepatuhanterhadapundang-undangtindakpidanakorupsi,fcpa,dan/atauabcdapatdilakukanolehauditorindependendenganketentuan:2.2.1.apabiladiinisiasiolehkkkscostrecovery,makaharusmendapatkanpersetujuanskkmigas;2.2.2.apabiladiinisiasiolehskkmigas,makaskkmigasakanmemberitahukandanmelibatkankkkscostrecovery;2.2.3.skkmigasataukkkscostrecoverymemberitahukankepadapelaksanakontrakmengenaiauditorindependenyangditunjuk,danpelaksanakontrakharusmenyampaikandatahardcopydandatadigitalkepadaauditorindependentersebut;dan2.2.4.biayapemeriksaandapatdibebankansebagaibiayaoperasiberdasarkankks.</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023sanksilampiranbabx1.pengawasanterhadapkkkscostrecovery1.2.sanksiataspelanggarandalampengelolaanpengadaanbarang/jasaberdasarkanhasilauditadalahsebagaiberikut:1.2.1.sanksiadministrasiberupasuratperingatankepadapimpinantertinggikkkscostrecovery,jika:1.2.1.1.tidakmelaksanakanprosespengelolaanpengadaanbarang/jasasesuaidenganketentuanpedomanini,petunjukpelaksanaanpengadaanbarang/jasa,dokumentender,dan/ataukontrak;1.2.2.sanksifinansialtidakdapatdibebankansebagaibiayaoperasiberdasarkankkspadaperiodeperhitunganberikutnyaatausetelahwilayahkerjakkkscostrecoverydalamtahapeksplorasidinyatakankomersialuntukdikembangkan,untuk:1.2.2.2.seluruhnilaikontrakyangterealisasi,jika:1.2.2.2.5.pelaksanakontraktidakbersediadilakukanauditkepatuhanterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dan/atauanti-briberyandcorruption(abc)untukpengadaanbarang/jasadarikontrakdimaksud.babxii3.apabilakkkscostrecoveryterbuktimelakukankelalaian,kesalahan,ataupelanggaranterhadapperaturanperundang-undanganyangberlaku,makakkkscostrecoverybertanggungjawabatassegalaakibathukumyangtimbuldanmelepaskan,membebaskan,danmembelaskkmigasdaridanterhadapsetiapkerugian,tuntutan,dangugatanhukumpihakketigasebagaiakibatdarikelalaian,kesalahan,ataupelanggarankewajibanhukumkkkscostrecoveryterhadapperaturanperundang-undanganyangberlaku.</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>c38307b641c2dac7b217f2111f1bd40651f88dc5a17df151d2db25d4c2f3bb06</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Memfasilitasi audit kepatuhan Kontraktor terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan Anti-bribery and Corruption (ABC)</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
+Kewajiban
+LAMPIRAN
+BAB X
+1. Pengawasan Terhadap KKKS Cost Recovery
+1.1. Pengawasan dilakukan oleh SKK Migas, auditor yang ditunjuk oleh SKK Migas, dan/atau auditor pemerintah secara pre, current, dan post audit terhadap seluruh rangkaian kegiatan pengelolaan Pengadaan Barang/Jasa sebagaimana diatur dalam pedoman ini, termasuk namun tidak terbatas pada kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan/atau Anti-Bribery and Corruption (ABC).
+1.2. Sanksi atas pelanggaran dalam pengelolaan Pengadaan Barang/Jasa berdasarkan hasil audit adalah sebagai berikut:
+1.2.2. Sanksi finansial
+Tidak dapat dibebankan sebagai biaya operasi berdasarkan KKS pada periode perhitungan berikutnya atau setelah wilayah kerja KKKS Cost Recovery dalam tahap eksplorasi dinyatakan komersial untuk dikembangkan, untuk:
+1.2.2.2. Seluruh nilai Kontrak yang terealisasi, jika:
+1.2.2.2.3. KKKS Cost Recovery tidak bersedia dilakukan audit kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan/atau Anti-Bribery and Corruption (ABC);</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
+Sanksi
+LAMPIRAN
+BAB X
+1. Pengawasan Terhadap KKKS Cost Recovery
+1.1. Pengawasan dilakukan oleh SKK Migas, auditor yang ditunjuk oleh SKK Migas, dan/atau auditor pemerintah secara pre, current, dan post audit terhadap seluruh rangkaian kegiatan pengelolaan Pengadaan Barang/Jasa sebagaimana diatur dalam pedoman ini, termasuk namun tidak terbatas pada kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan/atau Anti-Bribery and Corruption (ABC).
+1.2. Sanksi atas pelanggaran dalam pengelolaan Pengadaan Barang/Jasa berdasarkan hasil audit adalah sebagai berikut:
+1.2.2. Sanksi finansial
+Tidak dapat dibebankan sebagai biaya operasi berdasarkan KKS pada periode perhitungan berikutnya atau setelah wilayah kerja KKKS Cost Recovery dalam tahap eksplorasi dinyatakan komersial untuk dikembangkan, untuk:
+1.2.2.2. Seluruh nilai Kontrak yang terealisasi, jika:
+1.2.2.2.3. KKKS Cost Recovery tidak bersedia dilakukan audit kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan/atau Anti-Bribery and Corruption (ABC);
+BAB XII
+3. Apabila KKKS Cost Recovery terbukti melakukan kelalaian, kesalahan, atau pelanggaran terhadap Peraturan Perundang-Undangan yang berlaku, maka KKKS Cost Recovery bertanggung jawab atas segala akibat hukum yang timbul dan melepaskan, membebaskan, dan membela SKK Migas dari dan terhadap setiap kerugian, tuntutan, dan gugatan hukum pihak ketiga sebagai akibat dari kelalaian, kesalahan, atau pelanggaran kewajiban hukum KKKS Cost Recovery terhadap Peraturan Perundang-Undangan yang berlaku.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>memfasilitasiauditkepatuhankontraktorterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dananti-briberyandcorruption(abc)</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
         <is>
           <t>continuous</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>administratif</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>1.menyusundanmembiayaiprogrampendidikandanpelatihantenagakerjasetempatdan/ataunasional</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>peraturanpemerintahnomor96tahun2021kewajibanpasal161(1)pemegangiupdaniupkwajibmengutamakanpenggunaantenagakerjasetempat.(2)dalamhaltidaktersediatenagakerjasetempatsebagaimanadimaksudpadaayat(1)yangmemilikikompetensidankeahlian,pemegangiupdaniupkdapatmenggunakantenagakerjanasional.(3)dalamhaltidaktersediatenagakerjanasionaisebagainranadimaksudpadaayat(2)yangmemilikikompetensidankeahlian,pemegangiupdaniupkdapatmenggunakantenagakerjaasingsetelahmendapatkanpersetujuandariinstansiyangmenyelenggarakanurusanpemerintahandibidangketenagakerjaan.peraturanmenterienergidansumberdayamineralnomor25tahun2018kewajibanpasal29(1)pemegangiupeksplorasi,iupkeksplorasi,iupoperasiproduksi,iupkoperasiproduksi,iupoperasiproduksikhususuntukpengolahandan/ataupemurnian,danizinusahajasapertambanganwajibmengutamakantenagakerjasetempatdan/ataunasional.[...](3)pemegangiupeksplorasi,iupkeksplorasi,iupoperasiproduksi,iupkoperasiproduksi,iupoperasiproduksikhususuntukpengolahandan/ataupemurnian,danizinusahajasapertambanganwajibmenyusundanmembiayaiprogrampendidikandanpelatihantenagakerjasetempatdan/ataunasional.peraturanmenterienergidansumberdayamineralnomor39tahun2008kewajibanpasal3dalammelaksanakankegiatanusahapertambanganmineraldanbatubara,pemegangkuasapertambangan,pemegangkontrakkaryadanpemegangperjanjiankaryapengusahaanpertambanganbatubarawajibmempekerjakantenagakerjayangmemilikisertifikatkompetensikerjasesuaiskknisebagaimanadimaksuddalampasal1.</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>peraturanpemerintahnomor96tahun2021sanksipasal185(1)pemegangiup,iupk,ipr,sipb,atauiupuntukpenjualanyangmelakukanpelanggaranterhadapketentuansebagaimanadimaksuddalam[…]pasal161ayat(1)[…]dikenaisanksiadministratif.(2)sanksiadministratifsebagaimanadimaksudpadaayat(1)benrpa:a.peringatantertulis;b.penghentiansernentarasebagianatauseluruhkegiataneksplorasiatauoperasiproduksi;dan/atauc.pencabutaniup,iupk,ipr,sipb,atauiupuntukpenjualan.(3)selainsanksiadministratifsebagaimanadimaksudpadaayat(2),pemegangiup,iupk,ipr,atausipb,yangmelakukanpelanggaranterhadapketentuansebagaimanadimaksuddalampasal51ayat(2)hurufbdanpasal107ayat(2)hurufbdikenaidenda.(4)pengenaandendasebagaimanadimaksudpadaayat(3)dilaksanakansesuaidenganketentuanperaturanperundang-undangandibidangpajakdaerahdanretribusidaerah.pasal186peringatantertulissebagaimanadimaksuddalampasal185ayat(2)hurufadiberikanpalingbanyak3(tiga)kalidenganjangkawaktuperingatanmasing-masing30(tigapuluh)harikalender.peraturanmenterienergidansumberdayamineralnomor7tahun2020sanksipasal95(1)pemegangiup,iupk,iupoperasiproduksikhususuntukpengolahandan/ataupemurnian,iujp,daniupoperasiproduksikhususuntukpengangkutandanpenjualan,yangtidakmematuhiataumelanggarketentuansebagaimanadimaksuddalam[...]pasal72hurufaatauhurufm[...].(2)sanksiadministratifsebagaimanadimaksudpadaayat(1)berupa:a.peringatantertulis;b.penghentiansementarasebagianatauseluruhkegiatanusaha;dan/atauc.pencabutanizin.(3)sanksiadministratifsebagaimanadimaksudpadaayat(2)diberikanolehdirekturjenderalatasnamamenteriataugubernursesuaidengankewenangannya.peraturanmenterienergidansumberdayamineralnomor25tahun2018sanksipasal40(1)pemegangiupeksplorasi,iupkeksplorasi,iupoperasiproduksi,iupkoperasiproduksi,iupoperasiproduksikhususuntukpengolahandanataupemurnian,iupoperasiproduksikhususuntukpengangkutandanpenjualan,danizinusahajasapertambanganyangtidakmematuhiataumelanggarketentuansebagaimanadimaksuddalampasal8ayat(1)atausampaidenganayat(3),pasal9ayat(1),pasal10ayat(1),pasal11ayat(1),pasal12ayat(1),pasal13,pasal14ayat(1)atauayat(3),pasal16ayat(1)atauayat(6),pasal17ayat(1),pasal18ayat(1)atausampaidenganayat(6),pasal22,pasal24ayat(1)atauayat(3),pasal25ayat(1),pasal26ayat(1)atauayat(2),pasal27ayat(1),pasal29ayat(1)atauayat(3),pasal30ayat(1)atauayat(4),pasal33ayat(1),pasal38ayat(1),ayat(4),ayat(6),atauayat(7),ataupasal39ayat(1)dikenakansanksiadministratif.(2)sanksiadministratifsebagaimanadimaksudpadaayat(1)berupa:a.peringatantertulis;b.penghentiansementarasebagianatauseluruhkegiatanusaha;dan/atauc.pencabutanizin.(3)sanksiadministratifsebagaimanadimaksudpadaayat(2)diberikanolehdirekturjenderalatasnamamenteriataugubernursesuaidengankewenangannya.pasal41peringatantertulissebagaimanadimaksuddalampasal40ayat(2)hurufadiberikanpalingbanyak3(tiga)kalidenganjangkawaktuperingatanmasing-masingpalinglama30(tigapuluh)harikalender.pasal42(1)dalamhalpemegangiupeksplorasi,iupkeksplorasi,iupoperasiproduksi,iupkoperasiproduksi,iupoperasiproduksikhususuntukpengolahandan/ataupemurnian,iupoperasiproduksikhususuntukpengangkutandanpenjualan,atauizinusahajasapertambanganyangmendapatsanksiperingatantertulissetelahberakhirnyajangkawaktuperingatantertulissebagaimanadimaksuddalampasal40ayat(2)hurufabelummelaksanakankewajibannya,dikenakansanksiadministratifberupapenghentiansementarasebagianatauseluruhkegiatanusahasebagaimanadimaksuddalampasal40ayat(2)hurufb.(2)sanksiadministratifberupapenghentiansementarasebagianatauseluruhkegiatanusahasebagaimanadimaksudpadaayat(1)dikenakanpalinglama60(enampuluh)harikalender.pasal43sanksiadministratifberupapencabutanizinsebagaimanadimaksuddalampasal40ayat(2)hurufcdikenakankepadapemegangiupeksplorasi,iupkeksplorasi,iupoperasiproduksi,iupkoperasiproduksi,iupoperasiproduksikhususuntukpengolahandan/ataupemurnian,iupoperasiproduksikhususuntukpengangkutandanpenjualan,atauizinusahajasapertambanganyangtidakmelaksanakankewajibansampaidenganberakhirnyajangkawaktupengenaansanksiberupapenghentiansementarasebagianatauseluruhkegiatanusahasebagaimanadimaksuddalampasal42ayat(2)hurufb.</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>60067fe237909f5498f70c12409e0d2e803f203268213ed2839229c8999e1bf4</t>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023kewajibanlampiranbabx1.pengawasanterhadapkkkscostrecovery1.1.pengawasandilakukanolehskkmigas,auditoryangditunjukolehskkmigas,dan/atauauditorpemerintahsecarapre,current,danpostauditterhadapseluruhrangkaiankegiatanpengelolaanpengadaanbarang/jasasebagaimanadiaturdalampedomanini,termasuknamuntidakterbataspadakepatuhanterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dan/atauanti-briberyandcorruption(abc).1.2.sanksiataspelanggarandalampengelolaanpengadaanbarang/jasaberdasarkanhasilauditadalahsebagaiberikut:1.2.2.sanksifinansialtidakdapatdibebankansebagaibiayaoperasiberdasarkankkspadaperiodeperhitunganberikutnyaatausetelahwilayahkerjakkkscostrecoverydalamtahapeksplorasidinyatakankomersialuntukdikembangkan,untuk:1.2.2.2.seluruhnilaikontrakyangterealisasi,jika:1.2.2.2.3.kkkscostrecoverytidakbersediadilakukanauditkepatuhanterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dan/atauanti-briberyandcorruption(abc);</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023sanksilampiranbabx1.pengawasanterhadapkkkscostrecovery1.1.pengawasandilakukanolehskkmigas,auditoryangditunjukolehskkmigas,dan/atauauditorpemerintahsecarapre,current,danpostauditterhadapseluruhrangkaiankegiatanpengelolaanpengadaanbarang/jasasebagaimanadiaturdalampedomanini,termasuknamuntidakterbataspadakepatuhanterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dan/atauanti-briberyandcorruption(abc).1.2.sanksiataspelanggarandalampengelolaanpengadaanbarang/jasaberdasarkanhasilauditadalahsebagaiberikut:1.2.2.sanksifinansialtidakdapatdibebankansebagaibiayaoperasiberdasarkankkspadaperiodeperhitunganberikutnyaatausetelahwilayahkerjakkkscostrecoverydalamtahapeksplorasidinyatakankomersialuntukdikembangkan,untuk:1.2.2.2.seluruhnilaikontrakyangterealisasi,jika:1.2.2.2.3.kkkscostrecoverytidakbersediadilakukanauditkepatuhanterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dan/atauanti-briberyandcorruption(abc);babxii3.apabilakkkscostrecoveryterbuktimelakukankelalaian,kesalahan,ataupelanggaranterhadapperaturanperundang-undanganyangberlaku,makakkkscostrecoverybertanggungjawabatassegalaakibathukumyangtimbuldanmelepaskan,membebaskan,danmembelaskkmigasdaridanterhadapsetiapkerugian,tuntutan,dangugatanhukumpihakketigasebagaiakibatdarikelalaian,kesalahan,ataupelanggarankewajibanhukumkkkscostrecoveryterhadapperaturanperundang-undanganyangberlaku.</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>1e3ad0d8179e40d4bd6c008ca1402344f3e761f2d20625f66f58464b4c98626f</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Dilarang menandatangani Kontrak baru dengan Penyedia Barang/Jasa yang tidak bersedia untuk dilakukan audit kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi dan telah dikenakan sanksi oleh SKK Migas</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Prohibition</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
+Kewajiban
+LAMPIRAN
+BAB X
+1. Pengawasan Terhadap KKKS Cost Recovery
+1.1. Pengawasan dilakukan oleh SKK Migas, auditor yang ditunjuk oleh SKK Migas, dan/atau auditor pemerintah secara pre, current, dan post audit terhadap seluruh rangkaian kegiatan pengelolaan Pengadaan Barang/Jasa sebagaimana diatur dalam pedoman ini, termasuk namun tidak terbatas pada kepatuhan terhadap Undang-Undang Tindak Pidana Korupsi, Foreign Corrupt Practices Act (FCPA), dan/atau Anti-Bribery and Corruption (ABC).
+1.2. Sanksi atas pelanggaran dalam pengelolaan Pengadaan Barang/Jasa berdasarkan hasil audit adalah sebagai berikut:
+1.2.2. Sanksi finansial
+Tidak dapat dibebankan sebagai biaya operasi berdasarkan KKS pada periode perhitungan berikutnya atau setelah wilayah kerja KKKS Cost Recovery dalam tahap eksplorasi dinyatakan komersial untuk dikembangkan, untuk:
+1.2.2.2. Seluruh nilai Kontrak yang terealisasi, jika:
+1.2.2.2.4. KKKS Cost Recovery menandatangani Kontrak baru dengan Penyedia Barang/Jasa yang tidak bersedia dilakukan audit kepatuhan terhadap Undang-Undang Tipikor setelah penetapan sanksi oleh SKK Migas; atau</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e
+Sanksi
+LAMPIRAN
+BAB X
+1. Pengawasan Terhadap KKKS Cost Recovery
+1.2. Sanksi atas pelanggaran dalam pengelolaan Pengadaan Barang/Jasa berdasarkan hasil audit adalah sebagai berikut:
+1.2.1. Sanksi administrasi
+Berupa surat peringatan kepada pimpinan tertinggi KKKS Cost Recovery, jika:
+1.2.1.1. Tidak melaksanakan proses pengelolaan Pengadaan Barang/Jasa sesuai dengan ketentuan pedoman ini, Petunjuk Pelaksanaan Pengadaan Barang/Jasa, Dokumen Tender, dan/atau Kontrak;
+1.2.2. Sanksi finansial
+Tidak dapat dibebankan sebagai biaya operasi berdasarkan KKS pada periode perhitungan berikutnya atau setelah wilayah kerja KKKS Cost Recovery dalam tahap eksplorasi dinyatakan komersial untuk dikembangkan, untuk:
+1.2.2.2. Seluruh nilai Kontrak yang terealisasi, jika:
+1.2.2.2.4. KKKS Cost Recovery menandatangani Kontrak baru dengan Penyedia Barang/Jasa yang tidak bersedia dilakukan audit kepatuhan terhadap Undang-Undang Tipikor setelah penetapan sanksi oleh SKK Migas; atau
+BAB XII
+3. Apabila KKKS Cost Recovery terbukti melakukan kelalaian, kesalahan, atau pelanggaran terhadap Peraturan Perundang-Undangan yang berlaku, maka KKKS Cost Recovery bertanggung jawab atas segala akibat hukum yang timbul dan melepaskan, membebaskan, dan membela SKK Migas dari dan terhadap setiap kerugian, tuntutan, dan gugatan hukum pihak ketiga sebagai akibat dari kelalaian, kesalahan, atau pelanggaran kewajiban hukum KKKS Cost Recovery terhadap Peraturan Perundang-Undangan yang berlaku.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>dilarangmenandatanganikontrakbarudenganpenyediabarang/jasayangtidakbersediauntukdilakukanauditkepatuhanterhadapundang-undangtindakpidanakorupsidantelahdikenakansanksiolehskkmigas</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>prohibition</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023kewajibanlampiranbabx1.pengawasanterhadapkkkscostrecovery1.1.pengawasandilakukanolehskkmigas,auditoryangditunjukolehskkmigas,dan/atauauditorpemerintahsecarapre,current,danpostauditterhadapseluruhrangkaiankegiatanpengelolaanpengadaanbarang/jasasebagaimanadiaturdalampedomanini,termasuknamuntidakterbataspadakepatuhanterhadapundang-undangtindakpidanakorupsi,foreigncorruptpracticesact(fcpa),dan/atauanti-briberyandcorruption(abc).1.2.sanksiataspelanggarandalampengelolaanpengadaanbarang/jasaberdasarkanhasilauditadalahsebagaiberikut:1.2.2.sanksifinansialtidakdapatdibebankansebagaibiayaoperasiberdasarkankkspadaperiodeperhitunganberikutnyaatausetelahwilayahkerjakkkscostrecoverydalamtahapeksplorasidinyatakankomersialuntukdikembangkan,untuk:1.2.2.2.seluruhnilaikontrakyangterealisasi,jika:1.2.2.2.4.kkkscostrecoverymenandatanganikontrakbarudenganpenyediabarang/jasayangtidakbersediadilakukanauditkepatuhanterhadapundang-undangtipikorsetelahpenetapansanksiolehskkmigas;atau</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023sanksilampiranbabx1.pengawasanterhadapkkkscostrecovery1.2.sanksiataspelanggarandalampengelolaanpengadaanbarang/jasaberdasarkanhasilauditadalahsebagaiberikut:1.2.1.sanksiadministrasiberupasuratperingatankepadapimpinantertinggikkkscostrecovery,jika:1.2.1.1.tidakmelaksanakanprosespengelolaanpengadaanbarang/jasasesuaidenganketentuanpedomanini,petunjukpelaksanaanpengadaanbarang/jasa,dokumentender,dan/ataukontrak;1.2.2.sanksifinansialtidakdapatdibebankansebagaibiayaoperasiberdasarkankkspadaperiodeperhitunganberikutnyaatausetelahwilayahkerjakkkscostrecoverydalamtahapeksplorasidinyatakankomersialuntukdikembangkan,untuk:1.2.2.2.seluruhnilaikontrakyangterealisasi,jika:1.2.2.2.4.kkkscostrecoverymenandatanganikontrakbarudenganpenyediabarang/jasayangtidakbersediadilakukanauditkepatuhanterhadapundang-undangtipikorsetelahpenetapansanksiolehskkmigas;ataubabxii3.apabilakkkscostrecoveryterbuktimelakukankelalaian,kesalahan,ataupelanggaranterhadapperaturanperundang-undanganyangberlaku,makakkkscostrecoverybertanggungjawabatassegalaakibathukumyangtimbuldanmelepaskan,membebaskan,danmembelaskkmigasdaridanterhadapsetiapkerugian,tuntutan,dangugatanhukumpihakketigasebagaiakibatdarikelalaian,kesalahan,ataupelanggarankewajibanhukumkkkscostrecoveryterhadapperaturanperundang-undanganyangberlaku.</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>62a4d66d86b6c5bf5a4d649966ede3a51d86373eda4618b8f7d2f5759584a55b</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Menyampaikan Laporan Perubahan Lingkup Kontrak (PLK) per bulan kepada SKK Migas, paling lambat pada tanggal 5 (lima) bulan berikutnya</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Periodic</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>1. Menyampaikan melalui Sistem Informasi Pengelolaan Rantai Suplai (SI-PRS) SKK Migas.
+2. Mengacu pada format yang tercantum dalam Lampiran 13 Pedoman Tata Kerja Nomor 007/SKKMA0000/2017/S0 - Surat Keputusan Kepala SKK Migas Nomor KEP-0041/SKKMA0000/2017/S0 Tahun 2017.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>menyampaikanlaporanperubahanlingkupkontrak(plk)perbulankepadaskkmigas,palinglambatpadatanggal5(lima)bulanberikutnya</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>periodic</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>1.menyampaikanmelaluisisteminformasipengelolaanrantaisuplai(si-prs)skkmigas.2.mengacupadaformatyangtercantumdalamlampiran13pedomantatakerjanomor007/skkma0000/2017/s0-suratkeputusankepalaskkmigasnomorkep-0041/skkma0000/2017/s0tahun2017.</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>37e7f7870117c815ddaa6cba28f1ec8e2d8328d8c51460b991d6f56670a2c875</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Menyampaikan Laporan Tahunan kepada SKK Migas, dalam jangka waktu 2 (dua) minggu setelah periode yang akan dilaporkan berakhir</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Periodic</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Menyampaikan melalui Sistem Informasi Pengelolaan Rantai Suplai (SI-PRS) SKK Migas.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>menyampaikanlaporantahunankepadaskkmigas,dalamjangkawaktu2(dua)minggusetelahperiodeyangakandilaporkanberakhir</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>periodic</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>menyampaikanmelaluisisteminformasipengelolaanrantaisuplai(si-prs)skkmigas.</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>174a99c2ea20707ac0a0599699724e6b892e16fe70780cb2f5c89cda8e6228ea</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Menyampaikan Laporan Penutupan Kontrak dengan nilai lebih dari Rp5.000.000.000,00 (lima miliar rupiah) kepada SKK Migas, dalam jangka waktu 3 (tiga) minggu setelah seluruh hak dan kewajiban para pihak selesai dilaksanakan</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Continuous</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1. Menyampaikan melalui Sistem Informasi Pengelolaan Rantai Suplai (SI-PRS) SKK Migas.
+2. Melaporkan realisasi nilai Kontrak dan realisasi pencapaian Tingkat Komponen Dalam Negeri (TKDN) berdasarkan hasil verifikasi.</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>menyampaikanlaporanpenutupankontrakdengannilailebihdarirp5.000.000.000,00(limamiliarrupiah)kepadaskkmigas,dalamjangkawaktu3(tiga)minggusetelahseluruhhakdankewajibanparapihakselesaidilaksanakan</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>continuous</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>1.menyampaikanmelaluisisteminformasipengelolaanrantaisuplai(si-prs)skkmigas.2.melaporkanrealisasinilaikontrakdanrealisasipencapaiantingkatkomponendalamnegeri(tkdn)berdasarkanhasilverifikasi.</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>8eb7516a4ec7f8a831da61239b26ca42420b3bd07f0e0d78c23e5abc9b5b639a</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Menyampaikan Laporan Penunjukan Langsung Penyedia Barang/Jasa Afiliasi Badan Usaha Milik Negara (BUMN) oleh Kontraktor Afiliasi BUMN kepada SKK Migas secara berkala, paling sedikit 1 (satu) kali setahun</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Periodic</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Melaporkan dalam bentuk soft copy dan hard copy: a. realisasi upaya peningkatan efektivitas dan percepatan proses Pengadaan Barang/Jasa yang dilaksanakan; dan b. realisasi komitmen peningkatan kapabilitas, penambahan investasi dalam kepemilikan peralatan/fasilitas kerja, dan/atau penguasaan teknologi oleh Penyedia Barang/Jasa Afiliasi BUMN.</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>menyampaikanlaporanpenunjukanlangsungpenyediabarang/jasaafiliasibadanusahamiliknegara(bumn)olehkontraktorafiliasibumnkepadaskkmigassecaraberkala,palingsedikit1(satu)kalisetahun</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>periodic</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>melaporkandalambentuksoftcopydanhardcopy:a.realisasiupayapeningkatanefektivitasdanpercepatanprosespengadaanbarang/jasayangdilaksanakan;danb.realisasikomitmenpeningkatankapabilitas,penambahaninvestasidalamkepemilikanperalatan/fasilitaskerja,dan/ataupenguasaanteknologiolehpenyediabarang/jasaafiliasibumn.</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>e040eb4e5c26117a6f1b962f6eb8d6de8051d66ea43b5b79eb83875ef1c70d46</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Oil and Gas Procurement&gt;Pengadaan Barang dan Jasa dalam Kegiatan Usaha Hulu Minyak dan Gas Bumi</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Menyampaikan Laporan Tahunan untuk sanggahan banding yang ditembuskan kepada SKK Migas, dalam jangka waktu 2 (dua) minggu setelah periode yang akan dilaporkan berakhir</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Periodic</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Administratif</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Melaporkan dalam bentuk soft copy dan hard copy.</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Pedoman Tata Kerja Nomor PTK-007/SKKIA0000/2023/S9 - Surat Keputusan Kepala SKKMIGAS Nomor KEP-0042/SKKIA0000/2023/S9 Tahun 2023@lt64364e41f280e</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>menyampaikanlaporantahunanuntuksanggahanbandingyangditembuskankepadaskkmigas,dalamjangkawaktu2(dua)minggusetelahperiodeyangakandilaporkanberakhir</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>periodic</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>administratif</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>melaporkandalambentuksoftcopydanhardcopy.</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>pedomantatakerjanomorptk-007/skkia0000/2023/s9-suratkeputusankepalaskkmigasnomorkep-0042/skkia0000/2023/s9tahun2023</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>d2a1415f72eaa5e1ccc48dabda9e54f993f5e8d8f1e7e21e31bfc0ecca3431e8</t>
         </is>
       </c>
     </row>

</xml_diff>